<commit_message>
Fix: Group the session based on module and create actor-based venue assignment
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ModuleSem.xlsx
+++ b/src/main/resources/file/ModuleSem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA4AF907-FEFC-495B-BD9A-7AD3BC2218ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA571CEF-EAD3-447C-8F3B-58CDC693FD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Semester</t>
   </si>
@@ -54,18 +54,6 @@
   </si>
   <si>
     <t>ENG1044</t>
-  </si>
-  <si>
-    <t>OSS1014</t>
-  </si>
-  <si>
-    <t>PRG1203</t>
-  </si>
-  <si>
-    <t>SEG1201</t>
-  </si>
-  <si>
-    <t>WEB1201</t>
   </si>
 </sst>
 </file>
@@ -443,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9A3B3D-7D55-4B1C-B19D-1ADD38F7A84B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -495,38 +483,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrate student availability and assign them in group
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ModuleSem.xlsx
+++ b/src/main/resources/file/ModuleSem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA571CEF-EAD3-447C-8F3B-58CDC693FD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF48BD79-A6AC-4655-AFE9-E003F677E2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Schedule all student successfully
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ModuleSem.xlsx
+++ b/src/main/resources/file/ModuleSem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF48BD79-A6AC-4655-AFE9-E003F677E2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F278E657-DEAD-4E78-948E-8AA5CB7080B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Consider different semester and export timetable in excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ModuleSem.xlsx
+++ b/src/main/resources/file/ModuleSem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A5E4B1-6F8B-4494-959B-5B2B28405FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DAE6F0-8A30-4C1D-A457-775CCEDAFAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="3372" windowWidth="17280" windowHeight="8880" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Semester</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>ENG1044</t>
+  </si>
+  <si>
+    <t>SEG1201</t>
+  </si>
+  <si>
+    <t>OSS1014</t>
+  </si>
+  <si>
+    <t>WEB1201</t>
+  </si>
+  <si>
+    <t>PRG1203</t>
+  </si>
+  <si>
+    <t>NET1014</t>
   </si>
 </sst>
 </file>
@@ -431,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9A3B3D-7D55-4B1C-B19D-1ADD38F7A84B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B6" sqref="B6:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,6 +498,70 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactor minor problem and clear state
</commit_message>
<xml_diff>
--- a/src/main/resources/file/ModuleSem.xlsx
+++ b/src/main/resources/file/ModuleSem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wong zhao xuan\Documents\Programming Languages\Java\Course Timetable\timetable\src\main\resources\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BF6092-6235-4567-AF05-0116A849111E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DFF44-0853-4099-9965-5F6AC3A2459D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27480" yWindow="1620" windowWidth="21600" windowHeight="11235" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{30CCD6F0-C9D7-41E6-800B-2C2B61EC3410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Semester</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>MTH1114</t>
+  </si>
+  <si>
+    <t>SEG1201</t>
+  </si>
+  <si>
+    <t>OSS1014</t>
+  </si>
+  <si>
+    <t>WEB1201</t>
+  </si>
+  <si>
+    <t>PRG1203</t>
+  </si>
+  <si>
+    <t>ENG1044</t>
   </si>
   <si>
     <t>NET1014</t>
@@ -431,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9A3B3D-7D55-4B1C-B19D-1ADD38F7A84B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,7 +495,71 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>